<commit_message>
new graphs for sups ratings
</commit_message>
<xml_diff>
--- a/output/SpeakUpEvals.xlsx
+++ b/output/SpeakUpEvals.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14820" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Ratings" sheetId="2" r:id="rId1"/>
     <sheet name="Work Again" sheetId="3" r:id="rId2"/>
-    <sheet name="Absent" sheetId="4" r:id="rId3"/>
-    <sheet name="Additional Comments" sheetId="5" r:id="rId4"/>
-    <sheet name="Past Supervisors" sheetId="6" r:id="rId8"/>
+    <sheet name="Additional Comments" sheetId="5" r:id="rId3"/>
+    <sheet name="Past Supervisors" sheetId="6" r:id="rId4"/>
+    <sheet name="Absent" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0" fullCalcOnLoad="true" concurrentCalc="false"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="86">
   <si>
     <t>Supervisor</t>
   </si>
@@ -204,6 +204,84 @@
     <t>Too bossy</t>
   </si>
   <si>
+    <t>Additional Comments</t>
+  </si>
+  <si>
+    <t>She should improve on her communication about work plan</t>
+  </si>
+  <si>
+    <t>She is good leader and good to work with</t>
+  </si>
+  <si>
+    <t>She is a wonderful leader that i would wish to work with next time</t>
+  </si>
+  <si>
+    <t>She's very very very very very very good</t>
+  </si>
+  <si>
+    <t>I think it's all said!</t>
+  </si>
+  <si>
+    <t>He is short tampered. However he is a direct and honest guy.</t>
+  </si>
+  <si>
+    <t>I think he should work on being fast about communicating.</t>
+  </si>
+  <si>
+    <t>He should be considered for any future opportunities.</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>She is good to go.....It would be my pleasure if she remains a supervisor</t>
+  </si>
+  <si>
+    <t>She is friendly and has managed to pool contacts of many OC traffic officers</t>
+  </si>
+  <si>
+    <t>She is good for me</t>
+  </si>
+  <si>
+    <t>She is good and she loves what she does</t>
+  </si>
+  <si>
+    <t>She is the best</t>
+  </si>
+  <si>
+    <t>She's good and still good to be a supervisor incase of another project.</t>
+  </si>
+  <si>
+    <t>She was a good supervisor</t>
+  </si>
+  <si>
+    <t>Just fair.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  a beleiver, just like me. I like her.</t>
+  </si>
+  <si>
+    <t>Figures stress Julie.</t>
+  </si>
+  <si>
+    <t>She is good</t>
+  </si>
+  <si>
+    <t>Has a lot to improve</t>
+  </si>
+  <si>
+    <t>Which supervisors would you want to work under again?</t>
+  </si>
+  <si>
+    <t>How many people said they would want to work under the supervisor.</t>
+  </si>
+  <si>
+    <t>Lawrence</t>
+  </si>
+  <si>
+    <t>Godfrey</t>
+  </si>
+  <si>
     <t>How Many Times Absent</t>
   </si>
   <si>
@@ -211,84 +289,6 @@
   </si>
   <si>
     <t>How many times was your supervisor difficult to reach?</t>
-  </si>
-  <si>
-    <t>Additional Comments</t>
-  </si>
-  <si>
-    <t>She should improve on her communication about work plan</t>
-  </si>
-  <si>
-    <t>She is good leader and good to work with</t>
-  </si>
-  <si>
-    <t>She is a wonderful leader that i would wish to work with next time</t>
-  </si>
-  <si>
-    <t>She's very very very very very very good</t>
-  </si>
-  <si>
-    <t>I think it's all said!</t>
-  </si>
-  <si>
-    <t>He is short tampered. However he is a direct and honest guy.</t>
-  </si>
-  <si>
-    <t>I think he should work on being fast about communicating.</t>
-  </si>
-  <si>
-    <t>He should be considered for any future opportunities.</t>
-  </si>
-  <si>
-    <t>Good</t>
-  </si>
-  <si>
-    <t>She is good to go.....It would be my pleasure if she remains a supervisor</t>
-  </si>
-  <si>
-    <t>She is friendly and has managed to pool contacts of many OC traffic officers</t>
-  </si>
-  <si>
-    <t>She is good for me</t>
-  </si>
-  <si>
-    <t>She is good and she loves what she does</t>
-  </si>
-  <si>
-    <t>She is the best</t>
-  </si>
-  <si>
-    <t>She's good and still good to be a supervisor incase of another project.</t>
-  </si>
-  <si>
-    <t>She was a good supervisor</t>
-  </si>
-  <si>
-    <t>Just fair.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  a beleiver, just like me. I like her.</t>
-  </si>
-  <si>
-    <t>Figures stress Julie.</t>
-  </si>
-  <si>
-    <t>She is good</t>
-  </si>
-  <si>
-    <t>Has a lot to improve</t>
-  </si>
-  <si>
-    <t>Which supervisors would you want to work under again?</t>
-  </si>
-  <si>
-    <t>How many people said they would want to work under the supervisor.</t>
-  </si>
-  <si>
-    <t>Lawrence</t>
-  </si>
-  <si>
-    <t>Godfrey</t>
   </si>
 </sst>
 </file>
@@ -909,7 +909,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
@@ -925,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
@@ -933,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
@@ -941,7 +941,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
@@ -949,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.2">
@@ -965,7 +965,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.2">
@@ -973,7 +973,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.2">
@@ -981,7 +981,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.2">
@@ -989,7 +989,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.2">
@@ -997,7 +997,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.2">
@@ -1005,7 +1005,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.2">
@@ -1013,7 +1013,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.2">
@@ -1021,7 +1021,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.2">
@@ -1037,7 +1037,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.2">
@@ -1045,7 +1045,7 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.2">
@@ -1053,7 +1053,7 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.2">
@@ -1069,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" x14ac:dyDescent="0.2">
@@ -1077,7 +1077,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" x14ac:dyDescent="0.2">
@@ -1085,7 +1085,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" x14ac:dyDescent="0.2">
@@ -1101,7 +1101,7 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" x14ac:dyDescent="0.2">
@@ -1125,7 +1125,7 @@
         <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" x14ac:dyDescent="0.2">
@@ -1133,7 +1133,7 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1142,69 +1142,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="0">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -1217,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
@@ -1225,7 +1162,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
@@ -1241,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
@@ -1249,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
@@ -1257,7 +1194,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
@@ -1265,7 +1202,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.2">
@@ -1273,7 +1210,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.2">
@@ -1281,7 +1218,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.2">
@@ -1289,7 +1226,7 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.2">
@@ -1305,7 +1242,7 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.2">
@@ -1313,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.2">
@@ -1321,7 +1258,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.2">
@@ -1329,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" x14ac:dyDescent="0.2">
@@ -1337,7 +1274,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" x14ac:dyDescent="0.2">
@@ -1345,7 +1282,7 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" x14ac:dyDescent="0.2">
@@ -1353,7 +1290,7 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" x14ac:dyDescent="0.2">
@@ -1361,7 +1298,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" x14ac:dyDescent="0.2">
@@ -1369,7 +1306,7 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" x14ac:dyDescent="0.2">
@@ -1377,7 +1314,7 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" x14ac:dyDescent="0.2">
@@ -1385,7 +1322,97 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>81</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1395,84 +1422,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C6"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="5">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0">
         <v>2</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>